<commit_message>
merged per hand and exception handling in statistics
</commit_message>
<xml_diff>
--- a/04_Testing/05_Final_Release/TestReportOverview.xlsx
+++ b/04_Testing/05_Final_Release/TestReportOverview.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijal\Documents\Nachhilfeboerse\04_Testing\04_Tdot_Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Documents\GitHub\Nachhilfeboerse\04_Testing\05_Final_Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Test Report &lt;Project " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Test Report &lt;Project Name&gt;</t>
   </si>
@@ -53,11 +53,14 @@
   <si>
     <t>Jän 22, 2018</t>
   </si>
+  <si>
+    <t>Apr 16, 2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy"/>
   </numFmts>
@@ -152,7 +155,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -176,6 +179,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -263,7 +272,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -277,9 +286,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.5307599999999998E-2"/>
-          <c:y val="0.114221"/>
+          <c:y val="0.24651669342061266"/>
           <c:w val="0.93969199999999997"/>
-          <c:h val="0.85292800000000002"/>
+          <c:h val="0.72063222512286429"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -399,10 +408,13 @@
                 <c:pt idx="4">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FC27-48AC-8564-AF2BF4DA85BD}"/>
             </c:ext>
@@ -527,10 +539,13 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FC27-48AC-8564-AF2BF4DA85BD}"/>
             </c:ext>
@@ -655,10 +670,13 @@
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FC27-48AC-8564-AF2BF4DA85BD}"/>
             </c:ext>
@@ -674,11 +692,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="100"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:axId val="161930528"/>
+        <c:axId val="161923864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="161930528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,10 +727,10 @@
                 <a:latin typeface="Helvetica"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="161923864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,10 +738,10 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="161923864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -761,10 +779,10 @@
                 <a:latin typeface="Helvetica"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="161930528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -812,7 +830,7 @@
               <a:latin typeface="Helvetica"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -841,21 +859,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>154940</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>822960</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1979,7 +1997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1987,15 +2005,15 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.06640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="12.06640625" style="1" customWidth="1"/>
+    <col min="1" max="256" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2022,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="20.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2021,7 +2039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2039,7 +2057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -2074,7 +2092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2091,7 +2109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -2108,105 +2126,115 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+    <row r="8" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>

</xml_diff>